<commit_message>
Set match date to June 13, 2023 (the busiest day)
</commit_message>
<xml_diff>
--- a/backend/data/Matches.xlsx
+++ b/backend/data/Matches.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="94">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -284,6 +284,24 @@
   </si>
   <si>
     <t xml:space="preserve">Borna Coric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/06/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniil Medvedev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex de Minaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/06/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/06/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/06/18</t>
   </si>
 </sst>
 </file>
@@ -413,7 +431,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,6 +493,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,10 +631,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D74" activeCellId="0" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1487,6 +1509,380 @@
       </c>
       <c r="E51" s="0" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1503,7 +1899,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6 D14:E15 E16:E17 D17 D20">
+  <conditionalFormatting sqref="D14:E15 E16:E17 D17 D20 E6">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>TRUE()</formula>
     </cfRule>

</xml_diff>